<commit_message>
updated readme, flow sample metadata, and fixed error on flow stack
</commit_message>
<xml_diff>
--- a/data/flow_cell_samples/cell_list.xlsx
+++ b/data/flow_cell_samples/cell_list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lnkassa/Desktop/PNNL_synthetic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57ADBE42-F578-7749-A080-B056C02A8132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5226E6C-6B32-FF49-99BF-13276ADBCC39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="27040" yWindow="500" windowWidth="38400" windowHeight="19420" xr2:uid="{EA55358D-5091-D84E-BFA5-4E3F21CC7D4A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>file_id</t>
   </si>
@@ -105,9 +105,6 @@
   </si>
   <si>
     <t>csv</t>
-  </si>
-  <si>
-    <t>na</t>
   </si>
 </sst>
 </file>
@@ -497,7 +494,7 @@
   <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -571,45 +568,19 @@
       <c r="B2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="2">
-        <v>0</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" s="2">
-        <v>0</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" s="2">
-        <v>0</v>
-      </c>
-      <c r="L2" s="2">
-        <v>0</v>
-      </c>
-      <c r="M2" s="2">
-        <v>0</v>
-      </c>
-      <c r="N2" s="2">
-        <v>0</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>23</v>
-      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
       <c r="P2" s="2" t="s">
         <v>21</v>
       </c>

</xml_diff>